<commit_message>
sprite sheet and tile updated
forgot fast conveyor bend, added now
all chopshop ground tile print correctly
</commit_message>
<xml_diff>
--- a/Resources/Boards/ChopShop.xlsx
+++ b/Resources/Boards/ChopShop.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -51,9 +51,6 @@
     <t>convbl 180 1</t>
   </si>
   <si>
-    <t>convbr 180 2</t>
-  </si>
-  <si>
     <t>convhr 0 2</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>boardSpriteSheet.png</t>
+  </si>
+  <si>
+    <t>convbr 270 2</t>
   </si>
 </sst>
 </file>
@@ -521,16 +521,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="30.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="30.75" customHeight="1"/>
   <cols>
     <col min="1" max="12" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30.75" customHeight="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="50.25" customHeight="1">
@@ -538,16 +540,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>5</v>
@@ -556,45 +558,45 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="50.25" customHeight="1">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>2</v>
@@ -611,28 +613,28 @@
     </row>
     <row r="4" spans="1:12" ht="50.25" customHeight="1">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>2</v>
@@ -641,115 +643,115 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="50.25" customHeight="1">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="50.25" customHeight="1">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="50.25" customHeight="1">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>7</v>
@@ -769,98 +771,98 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
         <v>34</v>
       </c>
-      <c r="J8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" t="s">
-        <v>35</v>
-      </c>
       <c r="L8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="50.25" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="50.25" customHeight="1">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>38</v>
-      </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>8</v>
@@ -877,7 +879,7 @@
     </row>
     <row r="11" spans="1:12" ht="50.25" customHeight="1">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>2</v>
@@ -889,101 +891,101 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="50.25" customHeight="1">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" t="s">
-        <v>41</v>
-      </c>
       <c r="K12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="50.25" customHeight="1">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>1</v>
@@ -1001,7 +1003,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1013,7 +1015,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>